<commit_message>
purchased another cooler that is bigger and cheaper
</commit_message>
<xml_diff>
--- a/receipts/Purchases_Totals.xlsx
+++ b/receipts/Purchases_Totals.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juansalas/Desktop/SmartKoozie-1/receipts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yohan\Desktop\embeded\Project\SmartKoozie\receipts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E27109B-DEBB-E44B-8F32-79848482029D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{527822F1-2BBF-4269-B6F3-6D5DF06DDBA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{1B52948E-E76F-3B4D-BC34-59BD6D5B0CFF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1B52948E-E76F-3B4D-BC34-59BD6D5B0CFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Juan's purchases" sheetId="1" r:id="rId1"/>
     <sheet name="Robert's purchases" sheetId="2" r:id="rId2"/>
     <sheet name="Yohan's purchases" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
   <si>
     <t>Component</t>
   </si>
@@ -116,6 +116,18 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Peltier Cooler</t>
+  </si>
+  <si>
+    <t>TEC1-12706</t>
+  </si>
+  <si>
+    <t>Cooling</t>
+  </si>
+  <si>
+    <t>Yohan</t>
   </si>
 </sst>
 </file>
@@ -125,7 +137,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -138,6 +150,22 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -161,13 +189,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -502,20 +533,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B20EA56-24DF-AE4C-8E19-9258054FA0C2}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -533,7 +564,7 @@
       </c>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -550,7 +581,7 @@
         <v>35.46</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -567,7 +598,7 @@
         <v>10.66</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -584,7 +615,7 @@
         <v>10.69</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -601,7 +632,7 @@
         <v>22.97</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -616,7 +647,7 @@
       </c>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -631,7 +662,7 @@
       </c>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -648,7 +679,7 @@
         <v>4.2699999999999996</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -665,13 +696,30 @@
         <v>7.48</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="2">
+        <v>10.48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="2">
-        <f>SUM(E2:E9)</f>
-        <v>91.53</v>
+      <c r="E11" s="2">
+        <f>SUM(E2:E10)</f>
+        <v>102.01</v>
       </c>
     </row>
   </sheetData>
@@ -679,6 +727,7 @@
     <mergeCell ref="E5:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -690,14 +739,14 @@
       <selection activeCell="E5" sqref="E5:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -715,31 +764,31 @@
       </c>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
@@ -761,14 +810,14 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -786,31 +835,31 @@
       </c>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
bought a 40mm x 40mm x 20mm heat sink and added to excel sheet
</commit_message>
<xml_diff>
--- a/receipts/Purchases_Totals.xlsx
+++ b/receipts/Purchases_Totals.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yohan\Desktop\embeded\Project\SmartKoozie\receipts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{527822F1-2BBF-4269-B6F3-6D5DF06DDBA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B529FA55-5655-49F6-A952-DE069938C023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1B52948E-E76F-3B4D-BC34-59BD6D5B0CFF}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="31">
   <si>
     <t>Component</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>Yohan</t>
+  </si>
+  <si>
+    <t>heat transfer</t>
   </si>
 </sst>
 </file>
@@ -193,12 +196,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B20EA56-24DF-AE4C-8E19-9258054FA0C2}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -628,7 +631,7 @@
       <c r="D5" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="5">
         <v>22.97</v>
       </c>
     </row>
@@ -645,7 +648,7 @@
       <c r="D6" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -660,7 +663,7 @@
       <c r="D7" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="3"/>
+      <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -697,10 +700,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C10" t="s">
@@ -714,12 +717,26 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="2">
+        <v>9.6199999999999992</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="2">
-        <f>SUM(E2:E10)</f>
-        <v>102.01</v>
+      <c r="E12" s="2">
+        <f>SUM(E2:E11)</f>
+        <v>111.63000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -774,13 +791,13 @@
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E5" s="3"/>
+      <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E6" s="3"/>
+      <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E7" s="3"/>
+      <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E8" s="2"/>
@@ -845,13 +862,13 @@
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E5" s="3"/>
+      <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E6" s="3"/>
+      <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E7" s="3"/>
+      <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E8" s="2"/>

</xml_diff>

<commit_message>
Update purchase totals excel
</commit_message>
<xml_diff>
--- a/receipts/Purchases_Totals.xlsx
+++ b/receipts/Purchases_Totals.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yohan\Desktop\embeded\Project\SmartKoozie\receipts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juansalas/Desktop/SmartKoozie-1/receipts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E474BD4-3068-44A4-B474-98B511B7A397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{50926186-E427-8D4D-8C59-AA01ABBA1876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1B52948E-E76F-3B4D-BC34-59BD6D5B0CFF}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{1B52948E-E76F-3B4D-BC34-59BD6D5B0CFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Juan's purchases" sheetId="1" r:id="rId1"/>
     <sheet name="Robert's purchases" sheetId="2" r:id="rId2"/>
     <sheet name="Yohan's purchases" sheetId="3" r:id="rId3"/>
+    <sheet name="Totals" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="32">
   <si>
     <t>Component</t>
   </si>
@@ -128,6 +129,12 @@
   </si>
   <si>
     <t>Yohan</t>
+  </si>
+  <si>
+    <t>Robert</t>
+  </si>
+  <si>
+    <t>Even per person</t>
   </si>
 </sst>
 </file>
@@ -532,20 +539,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B20EA56-24DF-AE4C-8E19-9258054FA0C2}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
-    <col min="3" max="3" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -563,7 +570,7 @@
       </c>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -580,7 +587,7 @@
         <v>35.46</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -597,7 +604,7 @@
         <v>10.66</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -614,7 +621,7 @@
         <v>10.69</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -631,7 +638,7 @@
         <v>22.97</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -646,7 +653,7 @@
       </c>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -661,7 +668,7 @@
       </c>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -678,7 +685,7 @@
         <v>4.2699999999999996</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -695,33 +702,16 @@
         <v>7.48</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="2">
-        <v>10.48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="2">
-        <f>SUM(E2:E11)</f>
-        <v>102.01</v>
+      <c r="E11" s="2">
+        <f>SUM(E2:E9)</f>
+        <v>91.53</v>
       </c>
     </row>
   </sheetData>
@@ -741,14 +731,14 @@
       <selection activeCell="E5" sqref="E5:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
-    <col min="3" max="3" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -766,31 +756,31 @@
       </c>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
@@ -809,17 +799,17 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
-    <col min="3" max="3" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -837,35 +827,52 @@
       </c>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="2">
+        <v>10.48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E5" s="5"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="2"/>
+      <c r="E10" s="2">
+        <f>SUM(E2)</f>
+        <v>10.48</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -873,4 +880,67 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F127D262-AE98-0B4B-B15C-3D1CC4386962}">
+  <dimension ref="B3:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2">
+        <f>'Juan''s purchases'!E11</f>
+        <v>91.53</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="2">
+        <f>'Robert''s purchases'!E10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="2">
+        <f>'Yohan''s purchases'!E10</f>
+        <v>10.48</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="2">
+        <f>SUM(C3:C5)</f>
+        <v>102.01</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="2">
+        <f>C6/3</f>
+        <v>34.003333333333337</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>